<commit_message>
Cambios hasta registro exitoso de cliente
</commit_message>
<xml_diff>
--- a/DIAGRAMA DE BD PREVIO.xlsx
+++ b/DIAGRAMA DE BD PREVIO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tesis\Crizol\JoyeriaCrisol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="73">
   <si>
     <t>Foto</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>Contrasena</t>
+  </si>
+  <si>
+    <t>Clientes</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -451,15 +454,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -614,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -632,9 +626,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -642,72 +635,72 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,7 +1032,7 @@
   <dimension ref="A1:T49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,46 +1063,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="76" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="63" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="30" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="32" t="s">
+      <c r="A2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="31" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="4"/>
@@ -1122,369 +1115,368 @@
       <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="28"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="23" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="32" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
+      <c r="A4" s="44" t="s">
+        <v>8</v>
+      </c>
       <c r="E4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="65" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="33" t="s">
+      <c r="K4" s="32" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="82" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="81" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="66" t="s">
+      <c r="F5" s="27"/>
+      <c r="G5" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="P5" s="4"/>
     </row>
     <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="83" t="s">
+      <c r="A6" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="82" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="I6" s="22" t="s">
+      <c r="F6" s="27"/>
+      <c r="I6" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="33" t="s">
+      <c r="K6" s="32" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="28"/>
+      <c r="A7" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="27"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="67" t="s">
+      <c r="F7" s="27"/>
+      <c r="G7" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="K7" s="33" t="s">
+      <c r="K7" s="32" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="28"/>
+      <c r="A8" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="27"/>
       <c r="C8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="52" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="84" t="s">
+      <c r="A9" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="83" t="s">
         <v>47</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="28"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="K9" s="32" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="28"/>
+      <c r="A10" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="27"/>
       <c r="E10" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="24" t="s">
+      <c r="F10" s="27"/>
+      <c r="G10" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="53" t="s">
+      <c r="I10" s="52" t="s">
         <v>20</v>
       </c>
       <c r="J10" s="7"/>
-      <c r="K10" s="33" t="s">
+      <c r="K10" s="32" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="85" t="s">
+      <c r="A11" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="84" t="s">
         <v>62</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="69" t="s">
+      <c r="F11" s="27"/>
+      <c r="G11" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="54" t="s">
+      <c r="I11" s="53" t="s">
         <v>1</v>
       </c>
       <c r="J11" s="7"/>
-      <c r="K11" s="33" t="s">
+      <c r="K11" s="32" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="86" t="s">
+      <c r="A12" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="85" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="69" t="s">
+      <c r="F12" s="27"/>
+      <c r="G12" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="24" t="s">
         <v>5</v>
       </c>
       <c r="J12" s="7"/>
-      <c r="K12" s="35" t="s">
+      <c r="K12" s="34" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="28"/>
+      <c r="A13" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="27"/>
       <c r="C13" s="10" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="69" t="s">
+      <c r="F13" s="27"/>
+      <c r="G13" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="24" t="s">
         <v>6</v>
       </c>
       <c r="J13" s="7"/>
-      <c r="K13" s="33" t="s">
+      <c r="K13" s="32" t="s">
         <v>57</v>
       </c>
       <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="28"/>
+      <c r="A14" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="27"/>
       <c r="C14" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="70" t="s">
+      <c r="F14" s="27"/>
+      <c r="G14" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="I14" s="55" t="s">
+      <c r="I14" s="54" t="s">
         <v>9</v>
       </c>
       <c r="J14" s="7"/>
-      <c r="K14" s="33" t="s">
+      <c r="K14" s="32" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="87" t="s">
+      <c r="A15" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="86" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="K15" s="36" t="s">
+      <c r="F15" s="27"/>
+      <c r="K15" s="35" t="s">
         <v>59</v>
       </c>
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="E16" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="41"/>
+      <c r="I16" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="7"/>
+      <c r="K16" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="E16" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="71" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="42"/>
-      <c r="I16" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="88" t="s">
+      <c r="B17" s="27"/>
+      <c r="C17" s="87" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="42"/>
-      <c r="I17" s="57" t="s">
+      <c r="F17" s="27"/>
+      <c r="G17" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="41"/>
+      <c r="I17" s="56" t="s">
         <v>1</v>
       </c>
       <c r="J17" s="7"/>
-      <c r="K17" s="37" t="s">
+      <c r="K17" s="36" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="27" t="s">
+      <c r="A18" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="26" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="58" t="s">
+      <c r="F18" s="27"/>
+      <c r="G18" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="26" t="s">
+      <c r="H18" s="41"/>
+      <c r="I18" s="25" t="s">
         <v>5</v>
       </c>
       <c r="J18" s="7"/>
-      <c r="K18" s="17"/>
+      <c r="K18" s="16"/>
     </row>
     <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="28"/>
+      <c r="A19" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="27"/>
       <c r="C19" s="12" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="I19" s="58" t="s">
+      <c r="F19" s="27"/>
+      <c r="I19" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="42"/>
-      <c r="K19" s="38" t="s">
+      <c r="J19" s="41"/>
+      <c r="K19" s="37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="18" t="s">
-        <v>37</v>
+      <c r="A20" s="42" t="s">
+        <v>36</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="12" t="s">
@@ -1493,145 +1485,150 @@
       <c r="E20" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="73" t="s">
+      <c r="F20" s="27"/>
+      <c r="G20" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="39" t="s">
+      <c r="K20" s="38" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="89" t="s">
+      <c r="A21" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="88" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="74" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="59" t="s">
+      <c r="F21" s="27"/>
+      <c r="G21" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="40" t="s">
+      <c r="K21" s="39" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="43" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="28"/>
+      <c r="A22" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="27"/>
       <c r="E22" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="K22" s="41" t="s">
+      <c r="I22" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="40" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="90" t="s">
+      <c r="A23" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="28"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="20" t="s">
+      <c r="F23" s="27"/>
+      <c r="G23" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I23" s="61" t="s">
+      <c r="I23" s="60" t="s">
         <v>15</v>
       </c>
       <c r="J23" s="7"/>
-      <c r="K23" s="16"/>
+      <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="77" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="27"/>
+      <c r="G24" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="78" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="75" t="s">
+      <c r="B25" s="27"/>
+      <c r="C25" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="27"/>
+      <c r="E25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="I25" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="43" t="s">
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="92" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="I25" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="30"/>
+      <c r="C26" s="29"/>
       <c r="E26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="I26" s="30"/>
+      <c r="I26" s="29"/>
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="28"/>
+      <c r="A27" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="27"/>
       <c r="C27" s="2"/>
       <c r="E27" s="2"/>
       <c r="G27" s="2"/>
       <c r="I27" s="2"/>
       <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="28"/>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="27"/>
       <c r="C28" s="2"/>
       <c r="E28" s="2"/>
       <c r="G28" s="2"/>
       <c r="I28" s="2"/>
       <c r="K28" s="3"/>
     </row>
+    <row r="29" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="48" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>

</xml_diff>